<commit_message>
Documented USA_Functions, ROW_Functions, Arrays.py
</commit_message>
<xml_diff>
--- a/Include/All/can_pip_cap.xlsx
+++ b/Include/All/can_pip_cap.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\!Daniel\Programs\Pycharm\MODL\Include\All\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\OneDrive - Johns Hopkins University\Programs\Pycharm\MODL\Include\All\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{29C4F633-27B4-4221-AAD0-5CE1ABC35CA1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{29C4F633-27B4-4221-AAD0-5CE1ABC35CA1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{02ABA179-C99C-493F-8DC2-9B840574B217}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8952" xr2:uid="{72FBDB87-CBC6-4EAD-AD5D-1873B70EAAF3}"/>
   </bookViews>
@@ -21,7 +21,7 @@
   </externalReferences>
   <definedNames>
     <definedName name="region">#REF!</definedName>
-    <definedName name="region1">[2]Regions!$B$3:$C$61</definedName>
+    <definedName name="region1">[1]Regions!$B$3:$C$61</definedName>
     <definedName name="Regions">#REF!</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -106,9 +106,6 @@
   </si>
   <si>
     <t>Average Utilization Rate</t>
-  </si>
-  <si>
-    <t>Average annual Capacity (BCF/day)</t>
   </si>
   <si>
     <t>Average annual flows (BCF/day)</t>
@@ -296,6 +293,9 @@
       </rPr>
       <t>: Yukon, Northwest Territories, and Nunavut. All are in region CAW, but we choose Yukon as the "Region From"</t>
     </r>
+  </si>
+  <si>
+    <t>Capacity</t>
   </si>
 </sst>
 </file>
@@ -758,52 +758,13 @@
   </cellStyleXfs>
   <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -860,6 +821,45 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -880,6 +880,520 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Contents"/>
+      <sheetName val="Major Pipeline Summary"/>
+      <sheetName val="Inflow By Region"/>
+      <sheetName val="Outflow By Region"/>
+      <sheetName val="Region to Region Capacity Map"/>
+      <sheetName val="Inflow By State"/>
+      <sheetName val="Outflow By State"/>
+      <sheetName val="Inflow By State and Pipeline"/>
+      <sheetName val="Outflow By State and Pipeline"/>
+      <sheetName val="Pipeline State2State Capacity"/>
+      <sheetName val="Regions"/>
+      <sheetName val="Sheet1"/>
+      <sheetName val="Pipeline State2State CapacityH"/>
+      <sheetName val="InFlow Single Year"/>
+      <sheetName val="Outflow Single Year"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10">
+        <row r="3">
+          <cell r="B3" t="str">
+            <v>Alberta</v>
+          </cell>
+          <cell r="C3" t="str">
+            <v>Canada</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="B4" t="str">
+            <v>British Columbia</v>
+          </cell>
+          <cell r="C4" t="str">
+            <v>Canada</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="B5" t="str">
+            <v>Manitoba</v>
+          </cell>
+          <cell r="C5" t="str">
+            <v>Canada</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="B6" t="str">
+            <v>New Brunswick</v>
+          </cell>
+          <cell r="C6" t="str">
+            <v>Canada</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="B7" t="str">
+            <v>Ontario</v>
+          </cell>
+          <cell r="C7" t="str">
+            <v>Canada</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="B8" t="str">
+            <v>Quebec</v>
+          </cell>
+          <cell r="C8" t="str">
+            <v>Canada</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="B9" t="str">
+            <v>Saskatchewan</v>
+          </cell>
+          <cell r="C9" t="str">
+            <v>Canada</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="B10" t="str">
+            <v>Colorado</v>
+          </cell>
+          <cell r="C10" t="str">
+            <v>Central</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="B11" t="str">
+            <v>Iowa</v>
+          </cell>
+          <cell r="C11" t="str">
+            <v>Central</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="B12" t="str">
+            <v>Kansas</v>
+          </cell>
+          <cell r="C12" t="str">
+            <v>Central</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="B13" t="str">
+            <v>Missouri</v>
+          </cell>
+          <cell r="C13" t="str">
+            <v>Central</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="B14" t="str">
+            <v>Montana</v>
+          </cell>
+          <cell r="C14" t="str">
+            <v>Central</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="B15" t="str">
+            <v>Nebraska</v>
+          </cell>
+          <cell r="C15" t="str">
+            <v>Central</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="B16" t="str">
+            <v>North Dakota</v>
+          </cell>
+          <cell r="C16" t="str">
+            <v>Central</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="B17" t="str">
+            <v>South Dakota</v>
+          </cell>
+          <cell r="C17" t="str">
+            <v>Central</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="B18" t="str">
+            <v>Utah</v>
+          </cell>
+          <cell r="C18" t="str">
+            <v>Central</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="B19" t="str">
+            <v>Wyoming</v>
+          </cell>
+          <cell r="C19" t="str">
+            <v>Central</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="B20" t="str">
+            <v>Gulf of Mexico</v>
+          </cell>
+          <cell r="C20" t="str">
+            <v>Gulf of Mexico</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="B21" t="str">
+            <v>Gulf of Mexico - Deepwater</v>
+          </cell>
+          <cell r="C21" t="str">
+            <v>Gulf of Mexico</v>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="B22" t="str">
+            <v>Mexico</v>
+          </cell>
+          <cell r="C22" t="str">
+            <v>Mexico</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="B23" t="str">
+            <v>Illinois</v>
+          </cell>
+          <cell r="C23" t="str">
+            <v>Midwest</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="B24" t="str">
+            <v>Indiana</v>
+          </cell>
+          <cell r="C24" t="str">
+            <v>Midwest</v>
+          </cell>
+        </row>
+        <row r="25">
+          <cell r="B25" t="str">
+            <v>Michigan</v>
+          </cell>
+          <cell r="C25" t="str">
+            <v>Midwest</v>
+          </cell>
+        </row>
+        <row r="26">
+          <cell r="B26" t="str">
+            <v>Minnesota</v>
+          </cell>
+          <cell r="C26" t="str">
+            <v>Midwest</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="B27" t="str">
+            <v>Ohio</v>
+          </cell>
+          <cell r="C27" t="str">
+            <v>Midwest</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="B28" t="str">
+            <v>Wisconsin</v>
+          </cell>
+          <cell r="C28" t="str">
+            <v>Midwest</v>
+          </cell>
+        </row>
+        <row r="29">
+          <cell r="B29" t="str">
+            <v>Connecticut</v>
+          </cell>
+          <cell r="C29" t="str">
+            <v>Northeast</v>
+          </cell>
+        </row>
+        <row r="30">
+          <cell r="B30" t="str">
+            <v>Delaware</v>
+          </cell>
+          <cell r="C30" t="str">
+            <v>Northeast</v>
+          </cell>
+        </row>
+        <row r="31">
+          <cell r="B31" t="str">
+            <v>District of Columbia</v>
+          </cell>
+          <cell r="C31" t="str">
+            <v>Northeast</v>
+          </cell>
+        </row>
+        <row r="32">
+          <cell r="B32" t="str">
+            <v>Maine</v>
+          </cell>
+          <cell r="C32" t="str">
+            <v>Northeast</v>
+          </cell>
+        </row>
+        <row r="33">
+          <cell r="B33" t="str">
+            <v>Maryland</v>
+          </cell>
+          <cell r="C33" t="str">
+            <v>Northeast</v>
+          </cell>
+        </row>
+        <row r="34">
+          <cell r="B34" t="str">
+            <v>Massachusetts</v>
+          </cell>
+          <cell r="C34" t="str">
+            <v>Northeast</v>
+          </cell>
+        </row>
+        <row r="35">
+          <cell r="B35" t="str">
+            <v>New Hampshire</v>
+          </cell>
+          <cell r="C35" t="str">
+            <v>Northeast</v>
+          </cell>
+        </row>
+        <row r="36">
+          <cell r="B36" t="str">
+            <v>New Jersey</v>
+          </cell>
+          <cell r="C36" t="str">
+            <v>Northeast</v>
+          </cell>
+        </row>
+        <row r="37">
+          <cell r="B37" t="str">
+            <v>New York</v>
+          </cell>
+          <cell r="C37" t="str">
+            <v>Northeast</v>
+          </cell>
+        </row>
+        <row r="38">
+          <cell r="B38" t="str">
+            <v>Pennsylvania</v>
+          </cell>
+          <cell r="C38" t="str">
+            <v>Northeast</v>
+          </cell>
+        </row>
+        <row r="39">
+          <cell r="B39" t="str">
+            <v>Rhode Island</v>
+          </cell>
+          <cell r="C39" t="str">
+            <v>Northeast</v>
+          </cell>
+        </row>
+        <row r="40">
+          <cell r="B40" t="str">
+            <v>Vermont</v>
+          </cell>
+          <cell r="C40" t="str">
+            <v>Northeast</v>
+          </cell>
+        </row>
+        <row r="41">
+          <cell r="B41" t="str">
+            <v>Virginia</v>
+          </cell>
+          <cell r="C41" t="str">
+            <v>Northeast</v>
+          </cell>
+        </row>
+        <row r="42">
+          <cell r="B42" t="str">
+            <v>West Virginia</v>
+          </cell>
+          <cell r="C42" t="str">
+            <v>Northeast</v>
+          </cell>
+        </row>
+        <row r="43">
+          <cell r="B43" t="str">
+            <v>Alabama</v>
+          </cell>
+          <cell r="C43" t="str">
+            <v>Southeast</v>
+          </cell>
+        </row>
+        <row r="44">
+          <cell r="B44" t="str">
+            <v>Florida</v>
+          </cell>
+          <cell r="C44" t="str">
+            <v>Southeast</v>
+          </cell>
+        </row>
+        <row r="45">
+          <cell r="B45" t="str">
+            <v>Georgia</v>
+          </cell>
+          <cell r="C45" t="str">
+            <v>Southeast</v>
+          </cell>
+        </row>
+        <row r="46">
+          <cell r="B46" t="str">
+            <v>Kentucky</v>
+          </cell>
+          <cell r="C46" t="str">
+            <v>Southeast</v>
+          </cell>
+        </row>
+        <row r="47">
+          <cell r="B47" t="str">
+            <v>Mississippi</v>
+          </cell>
+          <cell r="C47" t="str">
+            <v>Southeast</v>
+          </cell>
+        </row>
+        <row r="48">
+          <cell r="B48" t="str">
+            <v>North Carolina</v>
+          </cell>
+          <cell r="C48" t="str">
+            <v>Southeast</v>
+          </cell>
+        </row>
+        <row r="49">
+          <cell r="B49" t="str">
+            <v>South Carolina</v>
+          </cell>
+          <cell r="C49" t="str">
+            <v>Southeast</v>
+          </cell>
+        </row>
+        <row r="50">
+          <cell r="B50" t="str">
+            <v>Tennessee</v>
+          </cell>
+          <cell r="C50" t="str">
+            <v>Southeast</v>
+          </cell>
+        </row>
+        <row r="51">
+          <cell r="B51" t="str">
+            <v>Arkansas</v>
+          </cell>
+          <cell r="C51" t="str">
+            <v>Southwest</v>
+          </cell>
+        </row>
+        <row r="52">
+          <cell r="B52" t="str">
+            <v>Louisiana</v>
+          </cell>
+          <cell r="C52" t="str">
+            <v>Southwest</v>
+          </cell>
+        </row>
+        <row r="53">
+          <cell r="B53" t="str">
+            <v>New Mexico</v>
+          </cell>
+          <cell r="C53" t="str">
+            <v>Southwest</v>
+          </cell>
+        </row>
+        <row r="54">
+          <cell r="B54" t="str">
+            <v>Oklahoma</v>
+          </cell>
+          <cell r="C54" t="str">
+            <v>Southwest</v>
+          </cell>
+        </row>
+        <row r="55">
+          <cell r="B55" t="str">
+            <v>Texas</v>
+          </cell>
+          <cell r="C55" t="str">
+            <v>Southwest</v>
+          </cell>
+        </row>
+        <row r="56">
+          <cell r="B56" t="str">
+            <v>Arizona</v>
+          </cell>
+          <cell r="C56" t="str">
+            <v>Western</v>
+          </cell>
+        </row>
+        <row r="57">
+          <cell r="B57" t="str">
+            <v>California</v>
+          </cell>
+          <cell r="C57" t="str">
+            <v>Western</v>
+          </cell>
+        </row>
+        <row r="58">
+          <cell r="B58" t="str">
+            <v>Idaho</v>
+          </cell>
+          <cell r="C58" t="str">
+            <v>Western</v>
+          </cell>
+        </row>
+        <row r="59">
+          <cell r="B59" t="str">
+            <v>Nevada</v>
+          </cell>
+          <cell r="C59" t="str">
+            <v>Western</v>
+          </cell>
+        </row>
+        <row r="60">
+          <cell r="B60" t="str">
+            <v>Oregon</v>
+          </cell>
+          <cell r="C60" t="str">
+            <v>Western</v>
+          </cell>
+        </row>
+        <row r="61">
+          <cell r="B61" t="str">
+            <v>Washington</v>
+          </cell>
+          <cell r="C61" t="str">
+            <v>Western</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -2004,520 +2518,6 @@
       <sheetData sheetId="59"/>
       <sheetData sheetId="60"/>
       <sheetData sheetId="61"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Contents"/>
-      <sheetName val="Major Pipeline Summary"/>
-      <sheetName val="Inflow By Region"/>
-      <sheetName val="Outflow By Region"/>
-      <sheetName val="Region to Region Capacity Map"/>
-      <sheetName val="Inflow By State"/>
-      <sheetName val="Outflow By State"/>
-      <sheetName val="Inflow By State and Pipeline"/>
-      <sheetName val="Outflow By State and Pipeline"/>
-      <sheetName val="Pipeline State2State Capacity"/>
-      <sheetName val="Regions"/>
-      <sheetName val="Sheet1"/>
-      <sheetName val="Pipeline State2State CapacityH"/>
-      <sheetName val="InFlow Single Year"/>
-      <sheetName val="Outflow Single Year"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10">
-        <row r="3">
-          <cell r="B3" t="str">
-            <v>Alberta</v>
-          </cell>
-          <cell r="C3" t="str">
-            <v>Canada</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="B4" t="str">
-            <v>British Columbia</v>
-          </cell>
-          <cell r="C4" t="str">
-            <v>Canada</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="B5" t="str">
-            <v>Manitoba</v>
-          </cell>
-          <cell r="C5" t="str">
-            <v>Canada</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="B6" t="str">
-            <v>New Brunswick</v>
-          </cell>
-          <cell r="C6" t="str">
-            <v>Canada</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="B7" t="str">
-            <v>Ontario</v>
-          </cell>
-          <cell r="C7" t="str">
-            <v>Canada</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="B8" t="str">
-            <v>Quebec</v>
-          </cell>
-          <cell r="C8" t="str">
-            <v>Canada</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="B9" t="str">
-            <v>Saskatchewan</v>
-          </cell>
-          <cell r="C9" t="str">
-            <v>Canada</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="B10" t="str">
-            <v>Colorado</v>
-          </cell>
-          <cell r="C10" t="str">
-            <v>Central</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="B11" t="str">
-            <v>Iowa</v>
-          </cell>
-          <cell r="C11" t="str">
-            <v>Central</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="B12" t="str">
-            <v>Kansas</v>
-          </cell>
-          <cell r="C12" t="str">
-            <v>Central</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="B13" t="str">
-            <v>Missouri</v>
-          </cell>
-          <cell r="C13" t="str">
-            <v>Central</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="B14" t="str">
-            <v>Montana</v>
-          </cell>
-          <cell r="C14" t="str">
-            <v>Central</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="B15" t="str">
-            <v>Nebraska</v>
-          </cell>
-          <cell r="C15" t="str">
-            <v>Central</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="B16" t="str">
-            <v>North Dakota</v>
-          </cell>
-          <cell r="C16" t="str">
-            <v>Central</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="B17" t="str">
-            <v>South Dakota</v>
-          </cell>
-          <cell r="C17" t="str">
-            <v>Central</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="B18" t="str">
-            <v>Utah</v>
-          </cell>
-          <cell r="C18" t="str">
-            <v>Central</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="B19" t="str">
-            <v>Wyoming</v>
-          </cell>
-          <cell r="C19" t="str">
-            <v>Central</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="B20" t="str">
-            <v>Gulf of Mexico</v>
-          </cell>
-          <cell r="C20" t="str">
-            <v>Gulf of Mexico</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="B21" t="str">
-            <v>Gulf of Mexico - Deepwater</v>
-          </cell>
-          <cell r="C21" t="str">
-            <v>Gulf of Mexico</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="B22" t="str">
-            <v>Mexico</v>
-          </cell>
-          <cell r="C22" t="str">
-            <v>Mexico</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="B23" t="str">
-            <v>Illinois</v>
-          </cell>
-          <cell r="C23" t="str">
-            <v>Midwest</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="B24" t="str">
-            <v>Indiana</v>
-          </cell>
-          <cell r="C24" t="str">
-            <v>Midwest</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="B25" t="str">
-            <v>Michigan</v>
-          </cell>
-          <cell r="C25" t="str">
-            <v>Midwest</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="B26" t="str">
-            <v>Minnesota</v>
-          </cell>
-          <cell r="C26" t="str">
-            <v>Midwest</v>
-          </cell>
-        </row>
-        <row r="27">
-          <cell r="B27" t="str">
-            <v>Ohio</v>
-          </cell>
-          <cell r="C27" t="str">
-            <v>Midwest</v>
-          </cell>
-        </row>
-        <row r="28">
-          <cell r="B28" t="str">
-            <v>Wisconsin</v>
-          </cell>
-          <cell r="C28" t="str">
-            <v>Midwest</v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="B29" t="str">
-            <v>Connecticut</v>
-          </cell>
-          <cell r="C29" t="str">
-            <v>Northeast</v>
-          </cell>
-        </row>
-        <row r="30">
-          <cell r="B30" t="str">
-            <v>Delaware</v>
-          </cell>
-          <cell r="C30" t="str">
-            <v>Northeast</v>
-          </cell>
-        </row>
-        <row r="31">
-          <cell r="B31" t="str">
-            <v>District of Columbia</v>
-          </cell>
-          <cell r="C31" t="str">
-            <v>Northeast</v>
-          </cell>
-        </row>
-        <row r="32">
-          <cell r="B32" t="str">
-            <v>Maine</v>
-          </cell>
-          <cell r="C32" t="str">
-            <v>Northeast</v>
-          </cell>
-        </row>
-        <row r="33">
-          <cell r="B33" t="str">
-            <v>Maryland</v>
-          </cell>
-          <cell r="C33" t="str">
-            <v>Northeast</v>
-          </cell>
-        </row>
-        <row r="34">
-          <cell r="B34" t="str">
-            <v>Massachusetts</v>
-          </cell>
-          <cell r="C34" t="str">
-            <v>Northeast</v>
-          </cell>
-        </row>
-        <row r="35">
-          <cell r="B35" t="str">
-            <v>New Hampshire</v>
-          </cell>
-          <cell r="C35" t="str">
-            <v>Northeast</v>
-          </cell>
-        </row>
-        <row r="36">
-          <cell r="B36" t="str">
-            <v>New Jersey</v>
-          </cell>
-          <cell r="C36" t="str">
-            <v>Northeast</v>
-          </cell>
-        </row>
-        <row r="37">
-          <cell r="B37" t="str">
-            <v>New York</v>
-          </cell>
-          <cell r="C37" t="str">
-            <v>Northeast</v>
-          </cell>
-        </row>
-        <row r="38">
-          <cell r="B38" t="str">
-            <v>Pennsylvania</v>
-          </cell>
-          <cell r="C38" t="str">
-            <v>Northeast</v>
-          </cell>
-        </row>
-        <row r="39">
-          <cell r="B39" t="str">
-            <v>Rhode Island</v>
-          </cell>
-          <cell r="C39" t="str">
-            <v>Northeast</v>
-          </cell>
-        </row>
-        <row r="40">
-          <cell r="B40" t="str">
-            <v>Vermont</v>
-          </cell>
-          <cell r="C40" t="str">
-            <v>Northeast</v>
-          </cell>
-        </row>
-        <row r="41">
-          <cell r="B41" t="str">
-            <v>Virginia</v>
-          </cell>
-          <cell r="C41" t="str">
-            <v>Northeast</v>
-          </cell>
-        </row>
-        <row r="42">
-          <cell r="B42" t="str">
-            <v>West Virginia</v>
-          </cell>
-          <cell r="C42" t="str">
-            <v>Northeast</v>
-          </cell>
-        </row>
-        <row r="43">
-          <cell r="B43" t="str">
-            <v>Alabama</v>
-          </cell>
-          <cell r="C43" t="str">
-            <v>Southeast</v>
-          </cell>
-        </row>
-        <row r="44">
-          <cell r="B44" t="str">
-            <v>Florida</v>
-          </cell>
-          <cell r="C44" t="str">
-            <v>Southeast</v>
-          </cell>
-        </row>
-        <row r="45">
-          <cell r="B45" t="str">
-            <v>Georgia</v>
-          </cell>
-          <cell r="C45" t="str">
-            <v>Southeast</v>
-          </cell>
-        </row>
-        <row r="46">
-          <cell r="B46" t="str">
-            <v>Kentucky</v>
-          </cell>
-          <cell r="C46" t="str">
-            <v>Southeast</v>
-          </cell>
-        </row>
-        <row r="47">
-          <cell r="B47" t="str">
-            <v>Mississippi</v>
-          </cell>
-          <cell r="C47" t="str">
-            <v>Southeast</v>
-          </cell>
-        </row>
-        <row r="48">
-          <cell r="B48" t="str">
-            <v>North Carolina</v>
-          </cell>
-          <cell r="C48" t="str">
-            <v>Southeast</v>
-          </cell>
-        </row>
-        <row r="49">
-          <cell r="B49" t="str">
-            <v>South Carolina</v>
-          </cell>
-          <cell r="C49" t="str">
-            <v>Southeast</v>
-          </cell>
-        </row>
-        <row r="50">
-          <cell r="B50" t="str">
-            <v>Tennessee</v>
-          </cell>
-          <cell r="C50" t="str">
-            <v>Southeast</v>
-          </cell>
-        </row>
-        <row r="51">
-          <cell r="B51" t="str">
-            <v>Arkansas</v>
-          </cell>
-          <cell r="C51" t="str">
-            <v>Southwest</v>
-          </cell>
-        </row>
-        <row r="52">
-          <cell r="B52" t="str">
-            <v>Louisiana</v>
-          </cell>
-          <cell r="C52" t="str">
-            <v>Southwest</v>
-          </cell>
-        </row>
-        <row r="53">
-          <cell r="B53" t="str">
-            <v>New Mexico</v>
-          </cell>
-          <cell r="C53" t="str">
-            <v>Southwest</v>
-          </cell>
-        </row>
-        <row r="54">
-          <cell r="B54" t="str">
-            <v>Oklahoma</v>
-          </cell>
-          <cell r="C54" t="str">
-            <v>Southwest</v>
-          </cell>
-        </row>
-        <row r="55">
-          <cell r="B55" t="str">
-            <v>Texas</v>
-          </cell>
-          <cell r="C55" t="str">
-            <v>Southwest</v>
-          </cell>
-        </row>
-        <row r="56">
-          <cell r="B56" t="str">
-            <v>Arizona</v>
-          </cell>
-          <cell r="C56" t="str">
-            <v>Western</v>
-          </cell>
-        </row>
-        <row r="57">
-          <cell r="B57" t="str">
-            <v>California</v>
-          </cell>
-          <cell r="C57" t="str">
-            <v>Western</v>
-          </cell>
-        </row>
-        <row r="58">
-          <cell r="B58" t="str">
-            <v>Idaho</v>
-          </cell>
-          <cell r="C58" t="str">
-            <v>Western</v>
-          </cell>
-        </row>
-        <row r="59">
-          <cell r="B59" t="str">
-            <v>Nevada</v>
-          </cell>
-          <cell r="C59" t="str">
-            <v>Western</v>
-          </cell>
-        </row>
-        <row r="60">
-          <cell r="B60" t="str">
-            <v>Oregon</v>
-          </cell>
-          <cell r="C60" t="str">
-            <v>Western</v>
-          </cell>
-        </row>
-        <row r="61">
-          <cell r="B61" t="str">
-            <v>Washington</v>
-          </cell>
-          <cell r="C61" t="str">
-            <v>Western</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -2823,907 +2823,907 @@
   <dimension ref="A1:Z40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="56.33203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.44140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="69.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="41.109375" style="6" customWidth="1"/>
-    <col min="8" max="8" width="28.5546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="34.88671875" style="6" customWidth="1"/>
-    <col min="10" max="10" width="34" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="35.109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.109375" style="38"/>
-    <col min="14" max="16384" width="9.109375" style="6"/>
+    <col min="1" max="1" width="6" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="56.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="69.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="41.109375" style="3" customWidth="1"/>
+    <col min="8" max="8" width="28.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="34.88671875" style="3" customWidth="1"/>
+    <col min="10" max="10" width="34" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="35.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.109375" style="25"/>
+    <col min="14" max="16384" width="9.109375" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="4" t="s">
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="59" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8"/>
-      <c r="O1" s="8"/>
-      <c r="P1" s="8"/>
-      <c r="Q1" s="8"/>
-      <c r="R1" s="8"/>
-      <c r="S1" s="8"/>
-      <c r="T1" s="8"/>
-      <c r="U1" s="8"/>
-      <c r="V1" s="8"/>
-      <c r="W1" s="8"/>
-      <c r="X1" s="8"/>
-      <c r="Y1" s="8"/>
-      <c r="Z1" s="9"/>
+      <c r="J1" s="59"/>
+      <c r="K1" s="59"/>
+      <c r="L1" s="59"/>
+      <c r="M1" s="59"/>
+      <c r="N1" s="59"/>
+      <c r="O1" s="59"/>
+      <c r="P1" s="59"/>
+      <c r="Q1" s="59"/>
+      <c r="R1" s="59"/>
+      <c r="S1" s="59"/>
+      <c r="T1" s="59"/>
+      <c r="U1" s="59"/>
+      <c r="V1" s="59"/>
+      <c r="W1" s="59"/>
+      <c r="X1" s="59"/>
+      <c r="Y1" s="59"/>
+      <c r="Z1" s="60"/>
     </row>
     <row r="2" spans="1:26" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="10"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="4" t="s">
+      <c r="A2" s="53"/>
+      <c r="B2" s="54"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="I2" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="8"/>
-      <c r="N2" s="8"/>
-      <c r="O2" s="8"/>
-      <c r="P2" s="8"/>
-      <c r="Q2" s="8"/>
-      <c r="R2" s="8"/>
-      <c r="S2" s="8"/>
-      <c r="T2" s="8"/>
-      <c r="U2" s="8"/>
-      <c r="V2" s="8"/>
-      <c r="W2" s="8"/>
-      <c r="X2" s="8"/>
-      <c r="Y2" s="8"/>
-      <c r="Z2" s="9"/>
+      <c r="J2" s="59"/>
+      <c r="K2" s="59"/>
+      <c r="L2" s="59"/>
+      <c r="M2" s="59"/>
+      <c r="N2" s="59"/>
+      <c r="O2" s="59"/>
+      <c r="P2" s="59"/>
+      <c r="Q2" s="59"/>
+      <c r="R2" s="59"/>
+      <c r="S2" s="59"/>
+      <c r="T2" s="59"/>
+      <c r="U2" s="59"/>
+      <c r="V2" s="59"/>
+      <c r="W2" s="59"/>
+      <c r="X2" s="59"/>
+      <c r="Y2" s="59"/>
+      <c r="Z2" s="60"/>
     </row>
     <row r="3" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="10"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="4" t="s">
+      <c r="A3" s="53"/>
+      <c r="B3" s="54"/>
+      <c r="C3" s="54"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="14" t="s">
+      <c r="I3" s="61" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
-      <c r="N3" s="14"/>
-      <c r="O3" s="14"/>
-      <c r="P3" s="14"/>
-      <c r="Q3" s="14"/>
-      <c r="R3" s="14"/>
-      <c r="S3" s="14"/>
-      <c r="T3" s="14"/>
-      <c r="U3" s="14"/>
-      <c r="V3" s="14"/>
-      <c r="W3" s="14"/>
-      <c r="X3" s="14"/>
-      <c r="Y3" s="14"/>
-      <c r="Z3" s="15"/>
+      <c r="J3" s="61"/>
+      <c r="K3" s="61"/>
+      <c r="L3" s="61"/>
+      <c r="M3" s="61"/>
+      <c r="N3" s="61"/>
+      <c r="O3" s="61"/>
+      <c r="P3" s="61"/>
+      <c r="Q3" s="61"/>
+      <c r="R3" s="61"/>
+      <c r="S3" s="61"/>
+      <c r="T3" s="61"/>
+      <c r="U3" s="61"/>
+      <c r="V3" s="61"/>
+      <c r="W3" s="61"/>
+      <c r="X3" s="61"/>
+      <c r="Y3" s="61"/>
+      <c r="Z3" s="62"/>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A4" s="10"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="4" t="s">
+      <c r="A4" s="53"/>
+      <c r="B4" s="54"/>
+      <c r="C4" s="54"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M4" s="6"/>
+      <c r="M4" s="3"/>
     </row>
     <row r="5" spans="1:26" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="16"/>
-      <c r="B5" s="17"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="4" t="s">
+      <c r="A5" s="56"/>
+      <c r="B5" s="57"/>
+      <c r="C5" s="57"/>
+      <c r="D5" s="58"/>
+      <c r="E5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="19">
+      <c r="F5" s="6">
         <v>2015</v>
       </c>
-      <c r="M5" s="6"/>
+      <c r="M5" s="3"/>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="M6" s="6"/>
+      <c r="M6" s="3"/>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A7" s="20"/>
-      <c r="B7" s="21" t="s">
+      <c r="A7" s="7"/>
+      <c r="B7" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="21" t="s">
+      <c r="C7" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="22" t="s">
+      <c r="D7" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="23" t="s">
+      <c r="E7" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="24" t="s">
+      <c r="F7" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="G7" s="25" t="s">
+      <c r="G7" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="H7" s="24" t="s">
+      <c r="H7" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="I7" s="23" t="s">
+      <c r="I7" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="J7" s="26" t="s">
+      <c r="J7" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="K7" s="26" t="s">
+      <c r="K7" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="L7" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="L7" s="27" t="s">
+      <c r="M7" s="15"/>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A8" s="16">
+        <v>1</v>
+      </c>
+      <c r="B8" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="M7" s="28"/>
-    </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A8" s="29">
-        <v>1</v>
-      </c>
-      <c r="B8" s="30" t="s">
+      <c r="C8" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="31" t="s">
+      <c r="D8" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="32" t="s">
+      <c r="E8" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="33" t="s">
-        <v>27</v>
-      </c>
-      <c r="F8" s="34" t="s">
-        <v>26</v>
-      </c>
-      <c r="G8" s="35"/>
-      <c r="H8" s="30" t="str">
-        <f>VLOOKUP(can_pip_cap!$E8,[1]nangam_regions!$AI$9:$AL$79,3,FALSE)</f>
+      <c r="F8" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8" s="22"/>
+      <c r="H8" s="17" t="str">
+        <f>VLOOKUP(can_pip_cap!$E8,[2]nangam_regions!$AI$9:$AL$79,3,FALSE)</f>
         <v>ENC</v>
       </c>
-      <c r="I8" s="20" t="str">
-        <f>VLOOKUP(can_pip_cap!$F8,[1]nangam_regions!$AI$9:$AL$79,3,FALSE)</f>
+      <c r="I8" s="7" t="str">
+        <f>VLOOKUP(can_pip_cap!$F8,[2]nangam_regions!$AI$9:$AL$79,3,FALSE)</f>
         <v>CAW</v>
       </c>
-      <c r="J8" s="36">
+      <c r="J8" s="23">
         <v>0.99</v>
       </c>
-      <c r="K8" s="36">
+      <c r="K8" s="23">
         <v>1.7</v>
       </c>
-      <c r="L8" s="37">
+      <c r="L8" s="24">
         <f>K8*J8</f>
         <v>1.6830000000000001</v>
       </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A9" s="39">
+      <c r="A9" s="26">
         <v>2</v>
       </c>
-      <c r="B9" s="34" t="s">
+      <c r="B9" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="31" t="s">
+      <c r="D9" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="38" t="s">
-        <v>26</v>
-      </c>
-      <c r="E9" s="33" t="s">
-        <v>30</v>
-      </c>
-      <c r="F9" s="34" t="s">
-        <v>26</v>
-      </c>
-      <c r="G9" s="40"/>
-      <c r="H9" s="34" t="str">
-        <f>VLOOKUP(can_pip_cap!$E9,[1]nangam_regions!$AI$9:$AL$79,3,FALSE)</f>
+      <c r="F9" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9" s="27"/>
+      <c r="H9" s="21" t="str">
+        <f>VLOOKUP(can_pip_cap!$E9,[2]nangam_regions!$AI$9:$AL$79,3,FALSE)</f>
         <v>CAW</v>
       </c>
-      <c r="I9" s="33" t="str">
-        <f>VLOOKUP(can_pip_cap!$F9,[1]nangam_regions!$AI$9:$AL$79,3,FALSE)</f>
+      <c r="I9" s="20" t="str">
+        <f>VLOOKUP(can_pip_cap!$F9,[2]nangam_regions!$AI$9:$AL$79,3,FALSE)</f>
         <v>CAW</v>
       </c>
-      <c r="J9" s="41">
+      <c r="J9" s="28">
         <v>0.65</v>
       </c>
-      <c r="K9" s="41">
+      <c r="K9" s="28">
         <v>2.9</v>
       </c>
-      <c r="L9" s="42">
+      <c r="L9" s="29">
         <f t="shared" ref="L9:L19" si="0">K9*J9</f>
         <v>1.885</v>
       </c>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A10" s="39">
+      <c r="A10" s="26">
         <v>2</v>
       </c>
-      <c r="B10" s="34" t="s">
+      <c r="B10" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="31" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" s="38" t="s">
-        <v>26</v>
-      </c>
-      <c r="E10" s="33" t="s">
-        <v>31</v>
-      </c>
-      <c r="F10" s="34" t="s">
-        <v>26</v>
-      </c>
-      <c r="G10" s="40"/>
-      <c r="H10" s="34" t="str">
-        <f>VLOOKUP(can_pip_cap!$E10,[1]nangam_regions!$AI$9:$AL$79,3,FALSE)</f>
+      <c r="D10" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10" s="27"/>
+      <c r="H10" s="21" t="str">
+        <f>VLOOKUP(can_pip_cap!$E10,[2]nangam_regions!$AI$9:$AL$79,3,FALSE)</f>
         <v>CAW</v>
       </c>
-      <c r="I10" s="33" t="str">
-        <f>VLOOKUP(can_pip_cap!$F10,[1]nangam_regions!$AI$9:$AL$79,3,FALSE)</f>
+      <c r="I10" s="20" t="str">
+        <f>VLOOKUP(can_pip_cap!$F10,[2]nangam_regions!$AI$9:$AL$79,3,FALSE)</f>
         <v>CAW</v>
       </c>
-      <c r="J10" s="41">
+      <c r="J10" s="28">
         <v>0.62</v>
       </c>
-      <c r="K10" s="41">
+      <c r="K10" s="28">
         <v>2.2000000000000002</v>
       </c>
-      <c r="L10" s="42">
+      <c r="L10" s="29">
         <f t="shared" si="0"/>
         <v>1.3640000000000001</v>
       </c>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A11" s="39">
+      <c r="A11" s="26">
         <v>3</v>
       </c>
-      <c r="B11" s="34" t="s">
+      <c r="B11" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="31" t="s">
+      <c r="D11" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="D11" s="38" t="s">
+      <c r="E11" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="E11" s="33" t="s">
-        <v>35</v>
-      </c>
-      <c r="F11" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="G11" s="40"/>
-      <c r="H11" s="34" t="str">
-        <f>VLOOKUP(can_pip_cap!$E11,[1]nangam_regions!$AI$9:$AL$79,3,FALSE)</f>
+      <c r="F11" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="G11" s="27"/>
+      <c r="H11" s="21" t="str">
+        <f>VLOOKUP(can_pip_cap!$E11,[2]nangam_regions!$AI$9:$AL$79,3,FALSE)</f>
         <v>CAE</v>
       </c>
-      <c r="I11" s="33" t="str">
-        <f>VLOOKUP(can_pip_cap!$F11,[1]nangam_regions!$AI$9:$AL$79,3,FALSE)</f>
+      <c r="I11" s="20" t="str">
+        <f>VLOOKUP(can_pip_cap!$F11,[2]nangam_regions!$AI$9:$AL$79,3,FALSE)</f>
         <v>CAE</v>
       </c>
-      <c r="J11" s="41">
+      <c r="J11" s="28">
         <v>0.45</v>
       </c>
-      <c r="K11" s="41">
+      <c r="K11" s="28">
         <v>0.56000000000000005</v>
       </c>
-      <c r="L11" s="42">
+      <c r="L11" s="29">
         <f t="shared" si="0"/>
         <v>0.25200000000000006</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A12" s="43">
+      <c r="A12" s="30">
         <v>4</v>
       </c>
-      <c r="B12" s="44" t="s">
+      <c r="B12" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="45" t="s">
-        <v>36</v>
-      </c>
-      <c r="D12" s="46" t="s">
+      <c r="E12" s="34" t="s">
+        <v>29</v>
+      </c>
+      <c r="F12" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="G12" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="E12" s="47" t="s">
-        <v>30</v>
-      </c>
-      <c r="F12" s="44" t="s">
-        <v>26</v>
-      </c>
-      <c r="G12" s="40" t="s">
-        <v>38</v>
-      </c>
-      <c r="H12" s="44" t="str">
-        <f>VLOOKUP(can_pip_cap!$E12,[1]nangam_regions!$AI$9:$AL$79,3,FALSE)</f>
+      <c r="H12" s="31" t="str">
+        <f>VLOOKUP(can_pip_cap!$E12,[2]nangam_regions!$AI$9:$AL$79,3,FALSE)</f>
         <v>CAW</v>
       </c>
-      <c r="I12" s="47" t="str">
-        <f>VLOOKUP(can_pip_cap!$F12,[1]nangam_regions!$AI$9:$AL$79,3,FALSE)</f>
+      <c r="I12" s="34" t="str">
+        <f>VLOOKUP(can_pip_cap!$F12,[2]nangam_regions!$AI$9:$AL$79,3,FALSE)</f>
         <v>CAW</v>
       </c>
-      <c r="J12" s="43">
+      <c r="J12" s="30">
         <v>0.97</v>
       </c>
-      <c r="K12" s="43">
+      <c r="K12" s="30">
         <v>8</v>
       </c>
-      <c r="L12" s="48">
+      <c r="L12" s="35">
         <f t="shared" si="0"/>
         <v>7.76</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A13" s="43">
+      <c r="A13" s="30">
         <v>4</v>
       </c>
-      <c r="B13" s="44" t="s">
+      <c r="B13" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="C13" s="45" t="s">
-        <v>36</v>
-      </c>
-      <c r="D13" s="46" t="s">
+      <c r="E13" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="F13" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="G13" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="E13" s="47" t="s">
-        <v>26</v>
-      </c>
-      <c r="F13" s="44" t="s">
-        <v>26</v>
-      </c>
-      <c r="G13" s="40" t="s">
-        <v>38</v>
-      </c>
-      <c r="H13" s="44" t="str">
-        <f>VLOOKUP(can_pip_cap!$E13,[1]nangam_regions!$AI$9:$AL$79,3,FALSE)</f>
+      <c r="H13" s="31" t="str">
+        <f>VLOOKUP(can_pip_cap!$E13,[2]nangam_regions!$AI$9:$AL$79,3,FALSE)</f>
         <v>CAW</v>
       </c>
-      <c r="I13" s="47" t="str">
-        <f>VLOOKUP(can_pip_cap!$F13,[1]nangam_regions!$AI$9:$AL$79,3,FALSE)</f>
+      <c r="I13" s="34" t="str">
+        <f>VLOOKUP(can_pip_cap!$F13,[2]nangam_regions!$AI$9:$AL$79,3,FALSE)</f>
         <v>CAW</v>
       </c>
-      <c r="J13" s="43">
+      <c r="J13" s="30">
         <v>0.72</v>
       </c>
-      <c r="K13" s="43">
+      <c r="K13" s="30">
         <v>4.3</v>
       </c>
-      <c r="L13" s="48">
+      <c r="L13" s="35">
         <f t="shared" si="0"/>
         <v>3.0959999999999996</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A14" s="43">
+      <c r="A14" s="30">
         <v>4</v>
       </c>
-      <c r="B14" s="44" t="s">
+      <c r="B14" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="C14" s="45" t="s">
-        <v>36</v>
-      </c>
-      <c r="D14" s="46" t="s">
+      <c r="E14" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="F14" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="G14" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="E14" s="47" t="s">
-        <v>26</v>
-      </c>
-      <c r="F14" s="44" t="s">
-        <v>26</v>
-      </c>
-      <c r="G14" s="40" t="s">
-        <v>38</v>
-      </c>
-      <c r="H14" s="44" t="str">
-        <f>VLOOKUP(can_pip_cap!$E14,[1]nangam_regions!$AI$9:$AL$79,3,FALSE)</f>
+      <c r="H14" s="31" t="str">
+        <f>VLOOKUP(can_pip_cap!$E14,[2]nangam_regions!$AI$9:$AL$79,3,FALSE)</f>
         <v>CAW</v>
       </c>
-      <c r="I14" s="47" t="str">
-        <f>VLOOKUP(can_pip_cap!$F14,[1]nangam_regions!$AI$9:$AL$79,3,FALSE)</f>
+      <c r="I14" s="34" t="str">
+        <f>VLOOKUP(can_pip_cap!$F14,[2]nangam_regions!$AI$9:$AL$79,3,FALSE)</f>
         <v>CAW</v>
       </c>
-      <c r="J14" s="43">
+      <c r="J14" s="30">
         <v>0.98</v>
       </c>
-      <c r="K14" s="43">
+      <c r="K14" s="30">
         <v>4.5</v>
       </c>
-      <c r="L14" s="48">
+      <c r="L14" s="35">
         <f t="shared" si="0"/>
         <v>4.41</v>
       </c>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A15" s="39">
+      <c r="A15" s="26">
         <v>5</v>
       </c>
-      <c r="B15" s="34" t="s">
+      <c r="B15" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="C15" s="31" t="s">
+      <c r="D15" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="D15" s="49" t="s">
+      <c r="E15" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="E15" s="33" t="s">
-        <v>42</v>
-      </c>
-      <c r="F15" s="34" t="s">
-        <v>42</v>
-      </c>
-      <c r="G15" s="40"/>
-      <c r="H15" s="34" t="str">
-        <f>VLOOKUP(can_pip_cap!$E15,[1]nangam_regions!$AI$9:$AL$79,3,FALSE)</f>
+      <c r="F15" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="G15" s="27"/>
+      <c r="H15" s="21" t="str">
+        <f>VLOOKUP(can_pip_cap!$E15,[2]nangam_regions!$AI$9:$AL$79,3,FALSE)</f>
         <v>CAE</v>
       </c>
-      <c r="I15" s="33" t="str">
-        <f>VLOOKUP(can_pip_cap!$F15,[1]nangam_regions!$AI$9:$AL$79,3,FALSE)</f>
+      <c r="I15" s="20" t="str">
+        <f>VLOOKUP(can_pip_cap!$F15,[2]nangam_regions!$AI$9:$AL$79,3,FALSE)</f>
         <v>CAE</v>
       </c>
-      <c r="J15" s="39">
+      <c r="J15" s="26">
         <v>0.62</v>
       </c>
-      <c r="K15" s="39">
+      <c r="K15" s="26">
         <v>0.8</v>
       </c>
-      <c r="L15" s="42">
+      <c r="L15" s="29">
         <f t="shared" si="0"/>
         <v>0.496</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A16" s="43">
+      <c r="A16" s="30">
         <v>6</v>
       </c>
-      <c r="B16" s="44" t="s">
+      <c r="B16" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="C16" s="50" t="s">
+      <c r="D16" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="D16" s="46" t="s">
+      <c r="E16" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="E16" s="47" t="s">
-        <v>46</v>
-      </c>
-      <c r="F16" s="44" t="s">
-        <v>26</v>
-      </c>
-      <c r="G16" s="51"/>
-      <c r="H16" s="44" t="str">
-        <f>VLOOKUP(can_pip_cap!$E16,[1]nangam_regions!$AI$9:$AL$79,3,FALSE)</f>
+      <c r="F16" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="G16" s="38"/>
+      <c r="H16" s="31" t="str">
+        <f>VLOOKUP(can_pip_cap!$E16,[2]nangam_regions!$AI$9:$AL$79,3,FALSE)</f>
         <v>CAE</v>
       </c>
-      <c r="I16" s="47" t="str">
-        <f>VLOOKUP(can_pip_cap!$F16,[1]nangam_regions!$AI$9:$AL$79,3,FALSE)</f>
+      <c r="I16" s="34" t="str">
+        <f>VLOOKUP(can_pip_cap!$F16,[2]nangam_regions!$AI$9:$AL$79,3,FALSE)</f>
         <v>CAW</v>
       </c>
-      <c r="J16" s="43">
+      <c r="J16" s="30">
         <v>0.43</v>
       </c>
-      <c r="K16" s="43">
+      <c r="K16" s="30">
         <v>6.9</v>
       </c>
-      <c r="L16" s="48">
+      <c r="L16" s="35">
         <f t="shared" si="0"/>
         <v>2.9670000000000001</v>
       </c>
     </row>
     <row r="17" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A17" s="43">
+      <c r="A17" s="30">
         <v>6</v>
       </c>
-      <c r="B17" s="44" t="s">
+      <c r="B17" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="C17" s="50" t="s">
-        <v>44</v>
-      </c>
-      <c r="D17" s="46" t="s">
+      <c r="D17" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="E17" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="F17" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="G17" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="E17" s="47" t="s">
-        <v>46</v>
-      </c>
-      <c r="F17" s="44" t="s">
-        <v>26</v>
-      </c>
-      <c r="G17" s="52" t="s">
-        <v>48</v>
-      </c>
-      <c r="H17" s="44" t="str">
-        <f>VLOOKUP(can_pip_cap!$E17,[1]nangam_regions!$AI$9:$AL$79,3,FALSE)</f>
+      <c r="H17" s="31" t="str">
+        <f>VLOOKUP(can_pip_cap!$E17,[2]nangam_regions!$AI$9:$AL$79,3,FALSE)</f>
         <v>CAE</v>
       </c>
-      <c r="I17" s="47" t="str">
-        <f>VLOOKUP(can_pip_cap!$F17,[1]nangam_regions!$AI$9:$AL$79,3,FALSE)</f>
+      <c r="I17" s="34" t="str">
+        <f>VLOOKUP(can_pip_cap!$F17,[2]nangam_regions!$AI$9:$AL$79,3,FALSE)</f>
         <v>CAW</v>
       </c>
-      <c r="J17" s="43">
+      <c r="J17" s="30">
         <v>0.6</v>
       </c>
-      <c r="K17" s="43">
+      <c r="K17" s="30">
         <v>3.6</v>
       </c>
-      <c r="L17" s="48">
+      <c r="L17" s="35">
         <f t="shared" si="0"/>
         <v>2.16</v>
       </c>
     </row>
     <row r="18" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A18" s="43">
+      <c r="A18" s="30">
         <v>6</v>
       </c>
-      <c r="B18" s="44" t="s">
+      <c r="B18" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="C18" s="50" t="s">
-        <v>44</v>
-      </c>
-      <c r="D18" s="46" t="s">
-        <v>49</v>
-      </c>
-      <c r="E18" s="47" t="s">
-        <v>46</v>
-      </c>
-      <c r="F18" s="44" t="s">
-        <v>46</v>
-      </c>
-      <c r="G18" s="51"/>
-      <c r="H18" s="44" t="str">
-        <f>VLOOKUP(can_pip_cap!$E18,[1]nangam_regions!$AI$9:$AL$79,3,FALSE)</f>
+      <c r="D18" s="33" t="s">
+        <v>48</v>
+      </c>
+      <c r="E18" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="F18" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="G18" s="38"/>
+      <c r="H18" s="31" t="str">
+        <f>VLOOKUP(can_pip_cap!$E18,[2]nangam_regions!$AI$9:$AL$79,3,FALSE)</f>
         <v>CAE</v>
       </c>
-      <c r="I18" s="47" t="str">
-        <f>VLOOKUP(can_pip_cap!$F18,[1]nangam_regions!$AI$9:$AL$79,3,FALSE)</f>
+      <c r="I18" s="34" t="str">
+        <f>VLOOKUP(can_pip_cap!$F18,[2]nangam_regions!$AI$9:$AL$79,3,FALSE)</f>
         <v>CAE</v>
       </c>
-      <c r="J18" s="43">
+      <c r="J18" s="30">
         <v>0.46</v>
       </c>
-      <c r="K18" s="43">
+      <c r="K18" s="30">
         <v>5.2</v>
       </c>
-      <c r="L18" s="48">
+      <c r="L18" s="35">
         <f t="shared" si="0"/>
         <v>2.3920000000000003</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="53">
+      <c r="A19" s="40">
         <v>7</v>
       </c>
-      <c r="B19" s="54" t="s">
+      <c r="B19" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="C19" s="42" t="s">
         <v>50</v>
       </c>
-      <c r="C19" s="55" t="s">
+      <c r="D19" s="43" t="s">
         <v>51</v>
       </c>
-      <c r="D19" s="56" t="s">
+      <c r="E19" s="44" t="s">
+        <v>29</v>
+      </c>
+      <c r="F19" s="41" t="s">
         <v>52</v>
       </c>
-      <c r="E19" s="57" t="s">
-        <v>30</v>
-      </c>
-      <c r="F19" s="54" t="s">
+      <c r="G19" s="45" t="s">
         <v>53</v>
       </c>
-      <c r="G19" s="58" t="s">
-        <v>54</v>
-      </c>
-      <c r="H19" s="54" t="str">
-        <f>VLOOKUP(can_pip_cap!$E19,[1]nangam_regions!$AI$9:$AL$79,3,FALSE)</f>
+      <c r="H19" s="41" t="str">
+        <f>VLOOKUP(can_pip_cap!$E19,[2]nangam_regions!$AI$9:$AL$79,3,FALSE)</f>
         <v>CAW</v>
       </c>
-      <c r="I19" s="57" t="str">
-        <f>VLOOKUP(can_pip_cap!$F19,[1]nangam_regions!$AI$9:$AL$79,3,FALSE)</f>
+      <c r="I19" s="44" t="str">
+        <f>VLOOKUP(can_pip_cap!$F19,[2]nangam_regions!$AI$9:$AL$79,3,FALSE)</f>
         <v>CAW</v>
       </c>
-      <c r="J19" s="53">
+      <c r="J19" s="40">
         <v>0.92</v>
       </c>
-      <c r="K19" s="53">
+      <c r="K19" s="40">
         <v>1.6</v>
       </c>
-      <c r="L19" s="59">
+      <c r="L19" s="46">
         <f t="shared" si="0"/>
         <v>1.4720000000000002</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A20" s="38"/>
-      <c r="B20" s="38"/>
-      <c r="C20" s="60"/>
-      <c r="D20" s="38"/>
-      <c r="E20" s="38"/>
-      <c r="F20" s="38"/>
-      <c r="G20" s="38"/>
-      <c r="H20" s="40"/>
-      <c r="I20" s="38"/>
-      <c r="J20" s="38"/>
-      <c r="K20" s="38"/>
-      <c r="L20" s="38"/>
+      <c r="A20" s="25"/>
+      <c r="B20" s="25"/>
+      <c r="C20" s="47"/>
+      <c r="D20" s="25"/>
+      <c r="E20" s="25"/>
+      <c r="F20" s="25"/>
+      <c r="G20" s="25"/>
+      <c r="H20" s="27"/>
+      <c r="I20" s="25"/>
+      <c r="J20" s="25"/>
+      <c r="K20" s="25"/>
+      <c r="L20" s="25"/>
     </row>
     <row r="21" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A21" s="38"/>
-      <c r="B21" s="38"/>
-      <c r="C21" s="60"/>
-      <c r="D21" s="38"/>
-      <c r="E21" s="38"/>
-      <c r="F21" s="38"/>
-      <c r="G21" s="38"/>
-      <c r="H21" s="40"/>
-      <c r="I21" s="38"/>
-      <c r="J21" s="38"/>
-      <c r="K21" s="38"/>
-      <c r="L21" s="38"/>
+      <c r="A21" s="25"/>
+      <c r="B21" s="25"/>
+      <c r="C21" s="47"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="25"/>
+      <c r="F21" s="25"/>
+      <c r="G21" s="25"/>
+      <c r="H21" s="27"/>
+      <c r="I21" s="25"/>
+      <c r="J21" s="25"/>
+      <c r="K21" s="25"/>
+      <c r="L21" s="25"/>
     </row>
     <row r="22" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A22" s="38"/>
-      <c r="B22" s="38"/>
-      <c r="C22" s="60"/>
-      <c r="D22" s="38"/>
-      <c r="J22" s="38"/>
-      <c r="K22" s="38"/>
-      <c r="L22" s="38"/>
+      <c r="A22" s="25"/>
+      <c r="B22" s="25"/>
+      <c r="C22" s="47"/>
+      <c r="D22" s="25"/>
+      <c r="J22" s="25"/>
+      <c r="K22" s="25"/>
+      <c r="L22" s="25"/>
     </row>
     <row r="23" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A23" s="4"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="61"/>
-      <c r="D23" s="4"/>
-      <c r="J23" s="4"/>
-      <c r="K23" s="4"/>
-      <c r="L23" s="38"/>
-      <c r="M23" s="4"/>
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="48"/>
+      <c r="D23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="25"/>
+      <c r="M23" s="1"/>
     </row>
     <row r="24" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A24" s="38"/>
-      <c r="B24" s="38"/>
-      <c r="C24" s="60"/>
-      <c r="D24" s="38"/>
-      <c r="J24" s="38"/>
-      <c r="K24" s="38"/>
-      <c r="L24" s="38"/>
+      <c r="A24" s="25"/>
+      <c r="B24" s="25"/>
+      <c r="C24" s="47"/>
+      <c r="D24" s="25"/>
+      <c r="J24" s="25"/>
+      <c r="K24" s="25"/>
+      <c r="L24" s="25"/>
     </row>
     <row r="25" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A25" s="38"/>
-      <c r="B25" s="38"/>
-      <c r="C25" s="60"/>
-      <c r="D25" s="38"/>
-      <c r="J25" s="38"/>
-      <c r="K25" s="38"/>
-      <c r="L25" s="38"/>
+      <c r="A25" s="25"/>
+      <c r="B25" s="25"/>
+      <c r="C25" s="47"/>
+      <c r="D25" s="25"/>
+      <c r="J25" s="25"/>
+      <c r="K25" s="25"/>
+      <c r="L25" s="25"/>
     </row>
     <row r="26" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A26" s="38"/>
-      <c r="B26" s="38"/>
-      <c r="C26" s="60"/>
-      <c r="D26" s="38"/>
-      <c r="J26" s="38"/>
-      <c r="K26" s="38"/>
-      <c r="L26" s="38"/>
+      <c r="A26" s="25"/>
+      <c r="B26" s="25"/>
+      <c r="C26" s="47"/>
+      <c r="D26" s="25"/>
+      <c r="J26" s="25"/>
+      <c r="K26" s="25"/>
+      <c r="L26" s="25"/>
     </row>
     <row r="27" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A27" s="38"/>
-      <c r="B27" s="38"/>
-      <c r="C27" s="60"/>
-      <c r="D27" s="38"/>
-      <c r="J27" s="38"/>
-      <c r="K27" s="38"/>
-      <c r="L27" s="38"/>
+      <c r="A27" s="25"/>
+      <c r="B27" s="25"/>
+      <c r="C27" s="47"/>
+      <c r="D27" s="25"/>
+      <c r="J27" s="25"/>
+      <c r="K27" s="25"/>
+      <c r="L27" s="25"/>
     </row>
     <row r="28" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A28" s="38"/>
-      <c r="B28" s="38"/>
-      <c r="C28" s="60"/>
-      <c r="D28" s="38"/>
-      <c r="J28" s="38"/>
-      <c r="K28" s="38"/>
-      <c r="L28" s="38"/>
+      <c r="A28" s="25"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="47"/>
+      <c r="D28" s="25"/>
+      <c r="J28" s="25"/>
+      <c r="K28" s="25"/>
+      <c r="L28" s="25"/>
     </row>
     <row r="29" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A29" s="38"/>
-      <c r="B29" s="38"/>
-      <c r="C29" s="60"/>
-      <c r="D29" s="38"/>
-      <c r="J29" s="38"/>
-      <c r="K29" s="38"/>
-      <c r="L29" s="38"/>
+      <c r="A29" s="25"/>
+      <c r="B29" s="25"/>
+      <c r="C29" s="47"/>
+      <c r="D29" s="25"/>
+      <c r="J29" s="25"/>
+      <c r="K29" s="25"/>
+      <c r="L29" s="25"/>
     </row>
     <row r="30" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A30" s="38"/>
-      <c r="B30" s="38"/>
-      <c r="C30" s="60"/>
-      <c r="D30" s="38"/>
-      <c r="J30" s="38"/>
-      <c r="K30" s="38"/>
-      <c r="L30" s="38"/>
+      <c r="A30" s="25"/>
+      <c r="B30" s="25"/>
+      <c r="C30" s="47"/>
+      <c r="D30" s="25"/>
+      <c r="J30" s="25"/>
+      <c r="K30" s="25"/>
+      <c r="L30" s="25"/>
     </row>
     <row r="31" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A31" s="38"/>
-      <c r="B31" s="38"/>
-      <c r="C31" s="60"/>
-      <c r="D31" s="38"/>
-      <c r="J31" s="38"/>
-      <c r="K31" s="38"/>
-      <c r="L31" s="38"/>
+      <c r="A31" s="25"/>
+      <c r="B31" s="25"/>
+      <c r="C31" s="47"/>
+      <c r="D31" s="25"/>
+      <c r="J31" s="25"/>
+      <c r="K31" s="25"/>
+      <c r="L31" s="25"/>
     </row>
     <row r="32" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A32" s="38"/>
-      <c r="B32" s="38"/>
-      <c r="C32" s="60"/>
-      <c r="D32" s="38"/>
-      <c r="J32" s="38"/>
-      <c r="K32" s="38"/>
-      <c r="L32" s="38"/>
+      <c r="A32" s="25"/>
+      <c r="B32" s="25"/>
+      <c r="C32" s="47"/>
+      <c r="D32" s="25"/>
+      <c r="J32" s="25"/>
+      <c r="K32" s="25"/>
+      <c r="L32" s="25"/>
     </row>
     <row r="33" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A33" s="38"/>
-      <c r="B33" s="38"/>
-      <c r="C33" s="60"/>
-      <c r="D33" s="38"/>
-      <c r="J33" s="38"/>
-      <c r="K33" s="38"/>
-      <c r="L33" s="38"/>
+      <c r="A33" s="25"/>
+      <c r="B33" s="25"/>
+      <c r="C33" s="47"/>
+      <c r="D33" s="25"/>
+      <c r="J33" s="25"/>
+      <c r="K33" s="25"/>
+      <c r="L33" s="25"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34" s="38"/>
-      <c r="B34" s="38"/>
-      <c r="C34" s="38"/>
-      <c r="D34" s="38"/>
-      <c r="J34" s="38"/>
-      <c r="K34" s="38"/>
-      <c r="L34" s="38"/>
+      <c r="A34" s="25"/>
+      <c r="B34" s="25"/>
+      <c r="C34" s="25"/>
+      <c r="D34" s="25"/>
+      <c r="J34" s="25"/>
+      <c r="K34" s="25"/>
+      <c r="L34" s="25"/>
     </row>
     <row r="35" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A35" s="38"/>
-      <c r="B35" s="38"/>
-      <c r="C35" s="60"/>
-      <c r="D35" s="38"/>
-      <c r="E35" s="38"/>
-      <c r="F35" s="38"/>
-      <c r="G35" s="38"/>
-      <c r="H35" s="40"/>
-      <c r="I35" s="38"/>
-      <c r="J35" s="38"/>
-      <c r="K35" s="38"/>
-      <c r="L35" s="38"/>
+      <c r="A35" s="25"/>
+      <c r="B35" s="25"/>
+      <c r="C35" s="47"/>
+      <c r="D35" s="25"/>
+      <c r="E35" s="25"/>
+      <c r="F35" s="25"/>
+      <c r="G35" s="25"/>
+      <c r="H35" s="27"/>
+      <c r="I35" s="25"/>
+      <c r="J35" s="25"/>
+      <c r="K35" s="25"/>
+      <c r="L35" s="25"/>
     </row>
     <row r="36" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A36" s="38"/>
-      <c r="B36" s="38"/>
-      <c r="C36" s="60"/>
-      <c r="D36" s="38"/>
-      <c r="E36" s="38"/>
-      <c r="F36" s="38"/>
-      <c r="G36" s="38"/>
-      <c r="H36" s="40"/>
-      <c r="I36" s="38"/>
-      <c r="J36" s="38"/>
-      <c r="K36" s="38"/>
-      <c r="L36" s="38"/>
+      <c r="A36" s="25"/>
+      <c r="B36" s="25"/>
+      <c r="C36" s="47"/>
+      <c r="D36" s="25"/>
+      <c r="E36" s="25"/>
+      <c r="F36" s="25"/>
+      <c r="G36" s="25"/>
+      <c r="H36" s="27"/>
+      <c r="I36" s="25"/>
+      <c r="J36" s="25"/>
+      <c r="K36" s="25"/>
+      <c r="L36" s="25"/>
     </row>
     <row r="37" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A37" s="38"/>
-      <c r="B37" s="38"/>
-      <c r="C37" s="60"/>
-      <c r="D37" s="38"/>
-      <c r="E37" s="38"/>
-      <c r="F37" s="38"/>
-      <c r="G37" s="38"/>
-      <c r="H37" s="40"/>
-      <c r="I37" s="38"/>
-      <c r="J37" s="38"/>
-      <c r="K37" s="38"/>
-      <c r="L37" s="38"/>
+      <c r="A37" s="25"/>
+      <c r="B37" s="25"/>
+      <c r="C37" s="47"/>
+      <c r="D37" s="25"/>
+      <c r="E37" s="25"/>
+      <c r="F37" s="25"/>
+      <c r="G37" s="25"/>
+      <c r="H37" s="27"/>
+      <c r="I37" s="25"/>
+      <c r="J37" s="25"/>
+      <c r="K37" s="25"/>
+      <c r="L37" s="25"/>
     </row>
     <row r="38" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A38" s="38"/>
-      <c r="B38" s="38"/>
-      <c r="C38" s="60"/>
-      <c r="D38" s="38"/>
-      <c r="E38" s="38"/>
-      <c r="F38" s="38"/>
-      <c r="G38" s="38"/>
-      <c r="H38" s="40"/>
-      <c r="I38" s="38"/>
-      <c r="J38" s="38"/>
-      <c r="K38" s="38"/>
-      <c r="L38" s="38"/>
+      <c r="A38" s="25"/>
+      <c r="B38" s="25"/>
+      <c r="C38" s="47"/>
+      <c r="D38" s="25"/>
+      <c r="E38" s="25"/>
+      <c r="F38" s="25"/>
+      <c r="G38" s="25"/>
+      <c r="H38" s="27"/>
+      <c r="I38" s="25"/>
+      <c r="J38" s="25"/>
+      <c r="K38" s="25"/>
+      <c r="L38" s="25"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A39" s="62"/>
-      <c r="B39" s="38"/>
-      <c r="C39" s="38"/>
-      <c r="D39" s="38"/>
-      <c r="E39" s="38"/>
-      <c r="F39" s="38"/>
-      <c r="G39" s="38"/>
-      <c r="H39" s="40"/>
-      <c r="I39" s="38"/>
-      <c r="J39" s="38"/>
-      <c r="K39" s="38"/>
-      <c r="L39" s="38"/>
+      <c r="A39" s="49"/>
+      <c r="B39" s="25"/>
+      <c r="C39" s="25"/>
+      <c r="D39" s="25"/>
+      <c r="E39" s="25"/>
+      <c r="F39" s="25"/>
+      <c r="G39" s="25"/>
+      <c r="H39" s="27"/>
+      <c r="I39" s="25"/>
+      <c r="J39" s="25"/>
+      <c r="K39" s="25"/>
+      <c r="L39" s="25"/>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A40" s="38"/>
-      <c r="B40" s="38"/>
-      <c r="C40" s="38"/>
-      <c r="D40" s="38"/>
-      <c r="E40" s="38"/>
-      <c r="F40" s="38"/>
-      <c r="G40" s="38"/>
-      <c r="H40" s="38"/>
-      <c r="I40" s="38"/>
-      <c r="J40" s="38"/>
-      <c r="K40" s="38"/>
-      <c r="L40" s="38"/>
+      <c r="A40" s="25"/>
+      <c r="B40" s="25"/>
+      <c r="C40" s="25"/>
+      <c r="D40" s="25"/>
+      <c r="E40" s="25"/>
+      <c r="F40" s="25"/>
+      <c r="G40" s="25"/>
+      <c r="H40" s="25"/>
+      <c r="I40" s="25"/>
+      <c r="J40" s="25"/>
+      <c r="K40" s="25"/>
+      <c r="L40" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>